<commit_message>
use proper values for dates in default values for xdate and xdatenillable
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="340" windowWidth="36220" windowHeight="17880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="16820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="178">
   <si>
     <t>text</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>xstringhidden</t>
+  </si>
+  <si>
+    <t>2014-08-01</t>
+  </si>
+  <si>
+    <t>2015-04-01</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -622,15 +628,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -644,6 +654,11 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -946,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5425,7 +5440,6 @@
     <hyperlink ref="W38" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5613,7 +5627,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5626,8 +5639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5991,8 +6004,8 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="4">
-        <v>41852</v>
+      <c r="H14" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -6014,8 +6027,8 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="4">
-        <v>42095</v>
+      <c r="H15" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:19">

</xml_diff>